<commit_message>
Update on 20200707 part 2
</commit_message>
<xml_diff>
--- a/文档/其他文档/Others/Sports/Formula One赛车比赛观赛选择方式.xlsx
+++ b/文档/其他文档/Others/Sports/Formula One赛车比赛观赛选择方式.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="观赛转播平台统计" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="81">
   <si>
     <t>第一次自由练习
 Free Practice 1</t>
@@ -362,6 +362,23 @@
   </si>
   <si>
     <t>Reddit集合网页直播</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://www.xiaomitv.net/tiyu/jinbaotiyu.html
+http://www.leshi123.com/tiyu/jinbaotiyu.html
+http://www.leshitya.com/tiyu/jinbaotiyu.html
+http://www.haoqu.net/3/shanghai/jinbty.html（高清）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>高清稳定，标清不稳定</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://www.xiaomitv.net/tiyu/wuxingtiyu.html
+http://www.leshi123.com/tiyu/wuxingtiyu.html
+https://www.feiliuzhibo.com/channel/wxty.html</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -543,9 +560,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -630,6 +644,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -641,12 +658,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -688,7 +708,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -723,7 +743,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -934,56 +954,56 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9" style="8"/>
-    <col min="7" max="7" width="15.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9" style="7"/>
+    <col min="7" max="7" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="25" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9" style="8"/>
-    <col min="12" max="12" width="21.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9" style="7"/>
+    <col min="12" max="12" width="21.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="25" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9" style="8"/>
-    <col min="15" max="15" width="11.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9" style="7"/>
+    <col min="15" max="15" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="9" style="1"/>
-    <col min="18" max="18" width="10.375" style="1" customWidth="1"/>
+    <col min="18" max="18" width="10.33203125" style="1" customWidth="1"/>
     <col min="19" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="3" t="s">
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="3" t="s">
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="M1" s="3"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="3" t="s">
+      <c r="M1" s="44"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="P1" s="3"/>
+      <c r="P1" s="44"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -1001,7 +1021,7 @@
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="18"/>
+      <c r="F2" s="17"/>
       <c r="G2" s="2" t="s">
         <v>14</v>
       </c>
@@ -1014,240 +1034,240 @@
       <c r="J2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K2" s="18"/>
+      <c r="K2" s="17"/>
       <c r="L2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="N2" s="18"/>
+      <c r="N2" s="17"/>
       <c r="O2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="P2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="W2" s="8"/>
-    </row>
-    <row r="3" spans="1:23" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="W2" s="7"/>
+    </row>
+    <row r="3" spans="1:23" ht="34.799999999999997" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="17"/>
-      <c r="G3" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="J3" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="K3" s="17"/>
-      <c r="L3" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="M3" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="N3" s="17"/>
-      <c r="O3" s="11" t="s">
+      <c r="B3" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="16"/>
+      <c r="G3" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" s="16"/>
+      <c r="L3" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="N3" s="16"/>
+      <c r="O3" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="P3" s="11" t="s">
+      <c r="P3" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="W3" s="8"/>
-    </row>
-    <row r="4" spans="1:23" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="W3" s="7"/>
+    </row>
+    <row r="4" spans="1:23" ht="34.799999999999997" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="17"/>
-      <c r="G4" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="J4" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="K4" s="17"/>
-      <c r="L4" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="M4" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="N4" s="17"/>
-      <c r="O4" s="11" t="s">
+      <c r="B4" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="16"/>
+      <c r="G4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" s="16"/>
+      <c r="L4" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="M4" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="N4" s="16"/>
+      <c r="O4" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="P4" s="11" t="s">
+      <c r="P4" s="10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:23" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:23" ht="34.799999999999997" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="17"/>
-      <c r="G5" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="I5" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="J5" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="K5" s="17"/>
-      <c r="L5" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="M5" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="N5" s="17"/>
-      <c r="O5" s="11" t="s">
+      <c r="B5" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="16"/>
+      <c r="G5" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="K5" s="16"/>
+      <c r="L5" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="M5" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="N5" s="16"/>
+      <c r="O5" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="P5" s="11" t="s">
+      <c r="P5" s="10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:23" ht="112.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="s">
+    <row r="6" spans="1:23" ht="104.4" x14ac:dyDescent="0.25">
+      <c r="A6" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="D6" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="22" t="s">
+      <c r="E6" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="F6" s="17"/>
-      <c r="G6" s="9" t="s">
+      <c r="F6" s="16"/>
+      <c r="G6" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="H6" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="I6" s="23" t="s">
+      <c r="I6" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="J6" s="22" t="s">
+      <c r="J6" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="K6" s="17"/>
-      <c r="L6" s="23" t="s">
+      <c r="K6" s="16"/>
+      <c r="L6" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="M6" s="22" t="s">
+      <c r="M6" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="N6" s="17"/>
-      <c r="O6" s="10" t="s">
+      <c r="N6" s="16"/>
+      <c r="O6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="P6" s="9" t="s">
+      <c r="P6" s="8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:23" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+    <row r="7" spans="1:23" ht="34.799999999999997" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="17"/>
-      <c r="G7" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="I7" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="J7" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="K7" s="17"/>
-      <c r="L7" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="M7" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="N7" s="17"/>
-      <c r="O7" s="10" t="s">
+      <c r="B7" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="16"/>
+      <c r="G7" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="K7" s="16"/>
+      <c r="L7" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="M7" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="N7" s="16"/>
+      <c r="O7" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="P7" s="9" t="s">
+      <c r="P7" s="8" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1269,19 +1289,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="17.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="50.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="29.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="17.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="74.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="29.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
@@ -1319,403 +1339,407 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="26" t="s">
+      <c r="A2" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="I2" s="25" t="s">
+      <c r="I2" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="J2" s="25" t="s">
+      <c r="J2" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="K2" s="25" t="s">
+      <c r="K2" s="24" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="28" t="s">
+      <c r="A3" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="I3" s="27" t="s">
+      <c r="I3" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="J3" s="27" t="s">
+      <c r="J3" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="K3" s="27" t="s">
+      <c r="K3" s="26" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29" t="s">
+      <c r="B4" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="J4" s="29" t="s">
+      <c r="J4" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="K4" s="29" t="s">
+      <c r="K4" s="28" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="30" t="s">
+    <row r="5" spans="1:11" ht="34.799999999999997" x14ac:dyDescent="0.25">
+      <c r="A5" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="G5" s="30" t="s">
+      <c r="B5" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="30"/>
-      <c r="I5" s="30" t="s">
+      <c r="H5" s="29"/>
+      <c r="I5" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="J5" s="31" t="s">
+      <c r="J5" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="K5" s="30" t="s">
+      <c r="K5" s="29" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="24" t="s">
+    <row r="6" spans="1:11" ht="52.2" x14ac:dyDescent="0.25">
+      <c r="A6" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="G6" s="6" t="s">
+      <c r="B6" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="H6" s="24"/>
-      <c r="I6" s="24" t="s">
+      <c r="H6" s="23"/>
+      <c r="I6" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="J6" s="6" t="s">
+      <c r="J6" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="K6" s="24" t="s">
+      <c r="K6" s="23" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="34" t="s">
+    <row r="7" spans="1:11" ht="87" x14ac:dyDescent="0.25">
+      <c r="A7" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="34"/>
-      <c r="C7" s="34" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34" t="s">
-        <v>32</v>
-      </c>
-      <c r="G7" s="35" t="s">
+      <c r="B7" s="33"/>
+      <c r="C7" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="H7" s="34"/>
-      <c r="I7" s="34" t="s">
+      <c r="H7" s="33"/>
+      <c r="I7" s="33" t="s">
         <v>73</v>
       </c>
-      <c r="J7" s="35" t="s">
+      <c r="J7" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="K7" s="34" t="s">
+      <c r="K7" s="33" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+    <row r="8" spans="1:11" ht="52.2" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="G8" s="33" t="s">
+      <c r="B8" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="32"/>
+      <c r="F8" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="G8" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="H8" s="33"/>
-      <c r="I8" s="33" t="s">
+      <c r="H8" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="I8" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="J8" s="5" t="s">
+      <c r="J8" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="K8" s="33" t="s">
+      <c r="K8" s="32" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+    <row r="9" spans="1:11" ht="69.599999999999994" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="G9" s="33" t="s">
+      <c r="B9" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="H9" s="33"/>
-      <c r="I9" s="33" t="s">
+      <c r="H9" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="I9" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="J9" s="5" t="s">
+      <c r="J9" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="K9" s="33" t="s">
+      <c r="K9" s="32" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="34.799999999999997" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="G10" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="H10" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="K10" s="23" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="34.799999999999997" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="H11" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="K11" s="23" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="34.799999999999997" x14ac:dyDescent="0.25">
+      <c r="A12" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="39"/>
+      <c r="F12" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" s="39"/>
+      <c r="H12" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="I12" s="39" t="s">
+        <v>73</v>
+      </c>
+      <c r="J12" s="38" t="s">
+        <v>68</v>
+      </c>
+      <c r="K12" s="39" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="34.799999999999997" x14ac:dyDescent="0.25">
+      <c r="A13" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" s="13"/>
+      <c r="G13" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="H13" s="37" t="s">
+        <v>58</v>
+      </c>
+      <c r="I13" s="36" t="s">
+        <v>75</v>
+      </c>
+      <c r="J13" s="36" t="s">
+        <v>69</v>
+      </c>
+      <c r="K13" s="13" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B10" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="G10" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="H10" s="32" t="s">
-        <v>51</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="J10" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="K10" s="24" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B11" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="G11" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="H11" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="I11" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="J11" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="K11" s="24" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="39" t="s">
-        <v>53</v>
-      </c>
-      <c r="B12" s="40" t="s">
-        <v>31</v>
-      </c>
-      <c r="C12" s="40" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" s="40" t="s">
-        <v>31</v>
-      </c>
-      <c r="E12" s="40"/>
-      <c r="F12" s="40" t="s">
-        <v>31</v>
-      </c>
-      <c r="G12" s="40"/>
-      <c r="H12" s="41" t="s">
-        <v>61</v>
-      </c>
-      <c r="I12" s="40" t="s">
-        <v>73</v>
-      </c>
-      <c r="J12" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="K12" s="40" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="37" t="s">
-        <v>46</v>
-      </c>
-      <c r="B13" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="F13" s="14"/>
-      <c r="G13" s="37" t="s">
+    <row r="14" spans="1:11" ht="52.2" x14ac:dyDescent="0.25">
+      <c r="A14" s="41" t="s">
+        <v>77</v>
+      </c>
+      <c r="B14" s="42" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="42" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="42" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="42" t="s">
+        <v>31</v>
+      </c>
+      <c r="F14" s="42"/>
+      <c r="G14" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="H13" s="38" t="s">
-        <v>58</v>
-      </c>
-      <c r="I13" s="37" t="s">
-        <v>75</v>
-      </c>
-      <c r="J13" s="37" t="s">
+      <c r="H14" s="43" t="s">
+        <v>59</v>
+      </c>
+      <c r="I14" s="42" t="s">
+        <v>71</v>
+      </c>
+      <c r="J14" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="K13" s="14" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A14" s="42" t="s">
-        <v>77</v>
-      </c>
-      <c r="B14" s="43" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="43" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" s="43" t="s">
-        <v>31</v>
-      </c>
-      <c r="E14" s="43" t="s">
-        <v>31</v>
-      </c>
-      <c r="F14" s="43"/>
-      <c r="G14" s="42" t="s">
-        <v>67</v>
-      </c>
-      <c r="H14" s="44" t="s">
-        <v>59</v>
-      </c>
-      <c r="I14" s="43" t="s">
-        <v>71</v>
-      </c>
-      <c r="J14" s="42" t="s">
-        <v>69</v>
-      </c>
-      <c r="K14" s="43" t="s">
+      <c r="K14" s="42" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1732,6 +1756,7 @@
     <hyperlink ref="H12" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
 
@@ -1741,7 +1766,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update on 20200707 part 3
</commit_message>
<xml_diff>
--- a/文档/其他文档/Others/Sports/Formula One赛车比赛观赛选择方式.xlsx
+++ b/文档/其他文档/Others/Sports/Formula One赛车比赛观赛选择方式.xlsx
@@ -378,7 +378,8 @@
   <si>
     <t>http://www.xiaomitv.net/tiyu/wuxingtiyu.html
 http://www.leshi123.com/tiyu/wuxingtiyu.html
-https://www.feiliuzhibo.com/channel/wxty.html</t>
+https://www.feiliuzhibo.com/channel/wxty.html
+http://www.haoqu.net/3/shanghai/wuxty.html （高清）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1514,7 +1515,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="52.2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="69.599999999999994" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>42</v>
       </c>
@@ -1544,7 +1545,7 @@
         <v>68</v>
       </c>
       <c r="K8" s="32" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="69.599999999999994" x14ac:dyDescent="0.25">

</xml_diff>